<commit_message>
project 3 write up
</commit_message>
<xml_diff>
--- a/ME7120_FEA/MatLab_FE_Code/WFEM_Brick/LbeamInput.xlsx
+++ b/ME7120_FEA/MatLab_FE_Code/WFEM_Brick/LbeamInput.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ado\Documents\GitHub\WSU_Classes\ME7120_FEA\MatLab_FE_Code\WFEM_Brick\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WSUadm\Documents\GitHub\WSU_Classes\ME7120_FEA\MatLab_FE_Code\WFEM_Brick\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23565" windowHeight="10380"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23565" windowHeight="10380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S52"/>
+  <dimension ref="A1:S105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D52"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2695,6 +2695,719 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>2</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0</v>
+      </c>
+      <c r="H56" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>3</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0</v>
+      </c>
+      <c r="H57" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>4</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>5</v>
+      </c>
+      <c r="B59" s="1">
+        <v>0</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0</v>
+      </c>
+      <c r="H59" s="1">
+        <f>SUM(H56:H58)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>6</v>
+      </c>
+      <c r="B60" s="1">
+        <v>0</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>7</v>
+      </c>
+      <c r="B61" s="1">
+        <v>0</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>8</v>
+      </c>
+      <c r="B62" s="1">
+        <v>0</v>
+      </c>
+      <c r="C62" s="1">
+        <v>1</v>
+      </c>
+      <c r="D62" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>9</v>
+      </c>
+      <c r="B63" s="1">
+        <v>0</v>
+      </c>
+      <c r="C63" s="1">
+        <v>1</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>10</v>
+      </c>
+      <c r="B64" s="1">
+        <v>0</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>11</v>
+      </c>
+      <c r="B65" s="1">
+        <v>0</v>
+      </c>
+      <c r="C65" s="1">
+        <v>1</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>12</v>
+      </c>
+      <c r="B66" s="1">
+        <v>0</v>
+      </c>
+      <c r="C66" s="1">
+        <v>1</v>
+      </c>
+      <c r="D66" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>13</v>
+      </c>
+      <c r="B67" s="1">
+        <v>0</v>
+      </c>
+      <c r="C67" s="1">
+        <v>1</v>
+      </c>
+      <c r="D67" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>14</v>
+      </c>
+      <c r="B68" s="1">
+        <v>0</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1</v>
+      </c>
+      <c r="D68" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>15</v>
+      </c>
+      <c r="B69" s="1">
+        <v>0</v>
+      </c>
+      <c r="C69" s="1">
+        <v>1</v>
+      </c>
+      <c r="D69" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>16</v>
+      </c>
+      <c r="B70" s="1">
+        <v>0</v>
+      </c>
+      <c r="C70" s="1">
+        <v>1</v>
+      </c>
+      <c r="D70" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>17</v>
+      </c>
+      <c r="B71" s="1">
+        <v>0</v>
+      </c>
+      <c r="C71" s="1">
+        <v>1</v>
+      </c>
+      <c r="D71" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>18</v>
+      </c>
+      <c r="B72" s="1">
+        <v>0</v>
+      </c>
+      <c r="C72" s="1">
+        <v>1</v>
+      </c>
+      <c r="D72" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>19</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1</v>
+      </c>
+      <c r="D73" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>20</v>
+      </c>
+      <c r="B74" s="1">
+        <v>0</v>
+      </c>
+      <c r="C74" s="1">
+        <v>1</v>
+      </c>
+      <c r="D74" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>21</v>
+      </c>
+      <c r="B75" s="1">
+        <v>0</v>
+      </c>
+      <c r="C75" s="1">
+        <v>1</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>22</v>
+      </c>
+      <c r="B76" s="1">
+        <v>0</v>
+      </c>
+      <c r="C76" s="1">
+        <v>1</v>
+      </c>
+      <c r="D76" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>23</v>
+      </c>
+      <c r="B77" s="1">
+        <v>0</v>
+      </c>
+      <c r="C77" s="1">
+        <v>1</v>
+      </c>
+      <c r="D77" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>24</v>
+      </c>
+      <c r="B78" s="1">
+        <v>0</v>
+      </c>
+      <c r="C78" s="1">
+        <v>1</v>
+      </c>
+      <c r="D78" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>25</v>
+      </c>
+      <c r="B79" s="1">
+        <v>0</v>
+      </c>
+      <c r="C79" s="1">
+        <v>1</v>
+      </c>
+      <c r="D79" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>26</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0</v>
+      </c>
+      <c r="C80" s="1">
+        <v>1</v>
+      </c>
+      <c r="D80" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>27</v>
+      </c>
+      <c r="B81" s="1">
+        <v>0</v>
+      </c>
+      <c r="C81" s="1">
+        <v>1</v>
+      </c>
+      <c r="D81" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>28</v>
+      </c>
+      <c r="B82" s="1">
+        <v>0</v>
+      </c>
+      <c r="C82" s="1">
+        <v>1</v>
+      </c>
+      <c r="D82" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>29</v>
+      </c>
+      <c r="B83" s="1">
+        <v>0</v>
+      </c>
+      <c r="C83" s="1">
+        <v>1</v>
+      </c>
+      <c r="D83" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>30</v>
+      </c>
+      <c r="B84" s="1">
+        <v>0</v>
+      </c>
+      <c r="C84" s="1">
+        <v>1</v>
+      </c>
+      <c r="D84" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>31</v>
+      </c>
+      <c r="B85" s="1">
+        <v>0</v>
+      </c>
+      <c r="C85" s="1">
+        <v>1</v>
+      </c>
+      <c r="D85" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>32</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0</v>
+      </c>
+      <c r="C86" s="1">
+        <v>1</v>
+      </c>
+      <c r="D86" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>33</v>
+      </c>
+      <c r="B87" s="1">
+        <v>0</v>
+      </c>
+      <c r="C87" s="1">
+        <v>1</v>
+      </c>
+      <c r="D87" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>34</v>
+      </c>
+      <c r="B88" s="1">
+        <v>0</v>
+      </c>
+      <c r="C88" s="1">
+        <v>1</v>
+      </c>
+      <c r="D88" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>35</v>
+      </c>
+      <c r="B89" s="1">
+        <v>0</v>
+      </c>
+      <c r="C89" s="1">
+        <v>1</v>
+      </c>
+      <c r="D89" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>36</v>
+      </c>
+      <c r="B90" s="1">
+        <v>0</v>
+      </c>
+      <c r="C90" s="1">
+        <v>1</v>
+      </c>
+      <c r="D90" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>37</v>
+      </c>
+      <c r="B91" s="1">
+        <v>0</v>
+      </c>
+      <c r="C91" s="1">
+        <v>1</v>
+      </c>
+      <c r="D91" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>38</v>
+      </c>
+      <c r="B92" s="1">
+        <v>0</v>
+      </c>
+      <c r="C92" s="1">
+        <v>1</v>
+      </c>
+      <c r="D92" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>39</v>
+      </c>
+      <c r="B93" s="1">
+        <v>0</v>
+      </c>
+      <c r="C93" s="1">
+        <v>1</v>
+      </c>
+      <c r="D93" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>40</v>
+      </c>
+      <c r="B94" s="1">
+        <v>0</v>
+      </c>
+      <c r="C94" s="1">
+        <v>1</v>
+      </c>
+      <c r="D94" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>41</v>
+      </c>
+      <c r="B95" s="1">
+        <v>0</v>
+      </c>
+      <c r="C95" s="1">
+        <v>1</v>
+      </c>
+      <c r="D95" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>42</v>
+      </c>
+      <c r="B96" s="1">
+        <v>0</v>
+      </c>
+      <c r="C96" s="1">
+        <v>1</v>
+      </c>
+      <c r="D96" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>43</v>
+      </c>
+      <c r="B97" s="1">
+        <v>0</v>
+      </c>
+      <c r="C97" s="1">
+        <v>1</v>
+      </c>
+      <c r="D97" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>44</v>
+      </c>
+      <c r="B98" s="1">
+        <v>0</v>
+      </c>
+      <c r="C98" s="1">
+        <v>1</v>
+      </c>
+      <c r="D98" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>45</v>
+      </c>
+      <c r="B99" s="1">
+        <v>0</v>
+      </c>
+      <c r="C99" s="1">
+        <v>1</v>
+      </c>
+      <c r="D99" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>46</v>
+      </c>
+      <c r="B100" s="1">
+        <v>0</v>
+      </c>
+      <c r="C100" s="1">
+        <v>1</v>
+      </c>
+      <c r="D100" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>47</v>
+      </c>
+      <c r="B101" s="1">
+        <v>0</v>
+      </c>
+      <c r="C101" s="1">
+        <v>1</v>
+      </c>
+      <c r="D101" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>48</v>
+      </c>
+      <c r="B102" s="1">
+        <v>0</v>
+      </c>
+      <c r="C102" s="1">
+        <v>1</v>
+      </c>
+      <c r="D102" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>49</v>
+      </c>
+      <c r="B103" s="1">
+        <v>0</v>
+      </c>
+      <c r="C103" s="1">
+        <v>1</v>
+      </c>
+      <c r="D103" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>50</v>
+      </c>
+      <c r="B104" s="1">
+        <v>0</v>
+      </c>
+      <c r="C104" s="1">
+        <v>1</v>
+      </c>
+      <c r="D104" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>51</v>
+      </c>
+      <c r="B105" s="1">
+        <v>0</v>
+      </c>
+      <c r="C105" s="1">
+        <v>1</v>
+      </c>
+      <c r="D105" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>